<commit_message>
[Change] Arjen and Rowan should learn more about advanced data structures.
</commit_message>
<xml_diff>
--- a/Team Docs/PeerReviewGlyn.xlsx
+++ b/Team Docs/PeerReviewGlyn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Y2\Block 3\Project startup\Team Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1ADA8B7A-C2C8-4C4C-8F3D-72D0A2738EFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72FAE28-3F8E-40BB-AD87-0CDEA9E9382B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -394,28 +394,30 @@
   </si>
   <si>
     <t>Strength(s):
-You work fast for prototyping with a focus on the priorities. You work with C# with expertise and efficiency. With C++ you don't shy away from challenge despite having mentioned that Engine dev and C++ is daunting. You ask for help when you need it and are willing to lend out a helping hand whenever it is needed. You get done what is needed.
-Improvement(s):
-Your understanding of more advanced C++ concepts can use improvement. If you're stuck with C++ you could ask for help sooner or for tips for research directions.</t>
-  </si>
-  <si>
-    <t>Strength(s):
 Skilled in C++ and engine development. Feels responsible for his tasks. Is willing to put in extra work when necessary. made improvements in trusting other programmers to implement sensitive systems.
 Improvement(s):
 Workload delegation, you could spread out your wokload more between the other programmers. Implementation time underestimation, despite adding 30% more implementation time you still manage to spend more time than the actual estimation. You should trust your fellow programmers more with intricate and complicated core systems. You tend to try to overcomplicate implementations for only a slightly bigger convenience for other team members, ask your temmembers to spend 5 seconds more instead of spending hours more yourself. Don't be a perfectionistic little bitch.</t>
+  </si>
+  <si>
+    <t>I keep getting stuck on no longer relevant topics during discussions, dragging out discussions unnecessarily. Should learn better time management.</t>
+  </si>
+  <si>
+    <t>I should rethink whether what I want to say is really still relevant. I should trust my fellow programmers with bigger tasks and add an even higher time margin to tasks.</t>
   </si>
   <si>
     <t>Strength(s):
 You deliver your work in a timely manner to the best of your abilities. Despite having daunting complicated tasks in an unknown engine and with a failry daunting unknown language you don't shy away from struggling through it anyways and delivering performance. You add a positive feel to the team.
 Improvement(s):
 C++ skills in more advanced topics could be improved. You lack confidence in your code. You are a good programmer, acknowledge that.
-You can spend more attention on being on time.</t>
+You can spend more attention on being on time.
+You should learn more about advanced data structures.</t>
   </si>
   <si>
-    <t>I keep getting stuck on no longer relevant topics during discussions, dragging out discussions unnecessarily. Should learn better time management.</t>
-  </si>
-  <si>
-    <t>I should rethink whether what I want to say is really still relevant. I should trust my fellow programmers with bigger tasks and add an even higher time margin to tasks.</t>
+    <t>Strength(s):
+You work fast for prototyping with a focus on the priorities. You work with C# with expertise and efficiency. With C++ you don't shy away from challenge despite having mentioned that Engine dev and C++ is daunting. You ask for help when you need it and are willing to lend out a helping hand whenever it is needed. You get done what is needed.
+Improvement(s):
+Your understanding of more advanced C++ concepts can use improvement. If you're stuck with C++ you could ask for help sooner or for tips for research directions.
+You should learn more about advanced data structures.</t>
   </si>
 </sst>
 </file>
@@ -1636,8 +1638,8 @@
   </sheetPr>
   <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z11" sqref="Z11"/>
+    <sheetView tabSelected="1" topLeftCell="J10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2240,19 +2242,19 @@
         <v>8</v>
       </c>
       <c r="J11" s="22" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="K11" s="24">
         <v>8</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M11" s="24">
         <v>7</v>
       </c>
       <c r="N11" s="22" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="O11" s="24">
         <v>8</v>
@@ -2275,10 +2277,10 @@
       <c r="W11" s="24"/>
       <c r="X11" s="25"/>
       <c r="Y11" s="26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="Z11" s="27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="100.2" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>